<commit_message>
fix misnamed things in excel
</commit_message>
<xml_diff>
--- a/Wartości.xlsx
+++ b/Wartości.xlsx
@@ -110,9 +110,6 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -124,6 +121,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -149,12 +149,9 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="pl-PL"/>
-              <a:t>Czasy rozwiązywania</a:t>
+              <a:t>Czasy dla zmiennej ilości kontenerów</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="pl-PL" baseline="0"/>
-              <a:t> problemu</a:t>
-            </a:r>
+            <a:endParaRPr lang="pl-PL" baseline="0"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -417,11 +414,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="91316224"/>
-        <c:axId val="91317760"/>
+        <c:axId val="124929920"/>
+        <c:axId val="124940672"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="91316224"/>
+        <c:axId val="124929920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -446,15 +443,16 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91317760"/>
+        <c:crossAx val="124940672"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="91317760"/>
+        <c:axId val="124940672"/>
         <c:scaling>
+          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
@@ -483,7 +481,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91316224"/>
+        <c:crossAx val="124929920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -496,7 +494,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -523,6 +521,15 @@
               <a:rPr lang="en-US"/>
               <a:t>łąd</a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="pl-PL"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pl-PL" sz="1800" b="1" i="0" u="none" strike="noStrike" baseline="0"/>
+              <a:t>dla zmiennej ilości kontenerów</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -659,11 +666,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="92127616"/>
-        <c:axId val="92129152"/>
+        <c:axId val="124957056"/>
+        <c:axId val="124958976"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="92127616"/>
+        <c:axId val="124957056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -692,14 +699,14 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92129152"/>
+        <c:crossAx val="124958976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="92129152"/>
+        <c:axId val="124958976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -730,7 +737,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92127616"/>
+        <c:crossAx val="124957056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -743,7 +750,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -753,6 +760,28 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="pl-PL"/>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL"/>
+              <a:t>Czasy dla zmiennej</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pl-PL" baseline="0"/>
+              <a:t> pojemności</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
@@ -1010,11 +1039,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="110106496"/>
-        <c:axId val="111808512"/>
+        <c:axId val="124423168"/>
+        <c:axId val="124425344"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="110106496"/>
+        <c:axId val="124423168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1030,11 +1059,11 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="pl-PL"/>
-                  <a:t>ilość</a:t>
+                  <a:t>pojemność</a:t>
                 </a:r>
                 <a:r>
                   <a:rPr lang="pl-PL" baseline="0"/>
-                  <a:t> kontenerów</a:t>
+                  <a:t> statku</a:t>
                 </a:r>
                 <a:endParaRPr lang="pl-PL"/>
               </a:p>
@@ -1044,15 +1073,16 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="111808512"/>
+        <c:crossAx val="124425344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="111808512"/>
+        <c:axId val="124425344"/>
         <c:scaling>
+          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
@@ -1077,7 +1107,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110106496"/>
+        <c:crossAx val="124423168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1090,7 +1120,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1101,6 +1131,21 @@
   <c:lang val="pl-PL"/>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL"/>
+              <a:t>Czasy dla zmiennej pojemności</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
     </c:title>
     <c:plotArea>
@@ -1234,11 +1279,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="41181568"/>
-        <c:axId val="41183104"/>
+        <c:axId val="124449536"/>
+        <c:axId val="124451456"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="41181568"/>
+        <c:axId val="124449536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1254,7 +1299,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="pl-PL"/>
-                  <a:t>ilość kontenerów</a:t>
+                  <a:t>pojemność statku</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1263,14 +1308,14 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="41183104"/>
+        <c:crossAx val="124451456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="41183104"/>
+        <c:axId val="124451456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1296,7 +1341,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="41181568"/>
+        <c:crossAx val="124449536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1309,7 +1354,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1727,8 +1772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O38" sqref="O38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1743,20 +1788,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="K1" s="1" t="s">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="K1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
     </row>
     <row r="2" spans="1:15">
       <c r="A2" t="s">
@@ -1785,392 +1830,392 @@
       </c>
     </row>
     <row r="3" spans="1:15">
-      <c r="A3" s="2">
+      <c r="A3" s="1">
         <v>20</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>1.9194499999866801</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>1.5700000076321802E-2</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="2">
         <v>0.87348810978966496</v>
       </c>
-      <c r="K3" s="2">
+      <c r="K3" s="1">
         <v>1000</v>
       </c>
-      <c r="L3" s="3">
+      <c r="L3" s="2">
         <v>1.0620000008202599</v>
       </c>
-      <c r="M3" s="3">
+      <c r="M3" s="2">
         <v>3.2850000570760998E-2</v>
       </c>
-      <c r="N3" s="3">
+      <c r="N3" s="2">
         <v>2.39857972833091</v>
       </c>
     </row>
     <row r="4" spans="1:15">
-      <c r="A4" s="4">
+      <c r="A4" s="3">
         <v>40</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="4">
         <v>3.2407999994757102</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="4">
         <v>1.6250001062871802E-2</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="4">
         <v>0.74711593966015799</v>
       </c>
-      <c r="K4" s="4">
+      <c r="K4" s="3">
         <v>2000</v>
       </c>
-      <c r="L4" s="5">
+      <c r="L4" s="4">
         <v>1.67615000013029</v>
       </c>
-      <c r="M4" s="5">
+      <c r="M4" s="4">
         <v>1.43499998375773E-2</v>
       </c>
-      <c r="N4" s="5">
+      <c r="N4" s="4">
         <v>1.4017394377365799</v>
       </c>
     </row>
     <row r="5" spans="1:15">
-      <c r="A5" s="2">
+      <c r="A5" s="1">
         <v>60</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="2">
         <v>4.7526499995728901</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>1.45999997039325E-2</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="2">
         <v>0.56756085577964199</v>
       </c>
-      <c r="K5" s="2">
+      <c r="K5" s="1">
         <v>3000</v>
       </c>
-      <c r="L5" s="3">
+      <c r="L5" s="2">
         <v>2.3985999998694698</v>
       </c>
-      <c r="M5" s="3">
+      <c r="M5" s="2">
         <v>1.09500001417472E-2</v>
       </c>
-      <c r="N5" s="3">
+      <c r="N5" s="2">
         <v>1.14761153253588</v>
       </c>
     </row>
     <row r="6" spans="1:15">
-      <c r="A6" s="4">
+      <c r="A6" s="3">
         <v>80</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="4">
         <v>6.4873500002431603</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="4">
         <v>1.99999994947575E-2</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="4">
         <v>0.47625454354459201</v>
       </c>
-      <c r="K6" s="4">
+      <c r="K6" s="3">
         <v>4000</v>
       </c>
-      <c r="L6" s="5">
+      <c r="L6" s="4">
         <v>3.3833999998750999</v>
       </c>
-      <c r="M6" s="5">
+      <c r="M6" s="4">
         <v>1.37500010896474E-2</v>
       </c>
-      <c r="N6" s="5">
+      <c r="N6" s="4">
         <v>0.80551225756905598</v>
       </c>
     </row>
     <row r="7" spans="1:15">
-      <c r="A7" s="2">
+      <c r="A7" s="1">
         <v>100</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="2">
         <v>8.8125999999465403</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="2">
         <v>2.45999998878687E-2</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="2">
         <v>0.37006572372123298</v>
       </c>
-      <c r="K7" s="2">
+      <c r="K7" s="1">
         <v>5000</v>
       </c>
-      <c r="L7" s="3">
+      <c r="L7" s="2">
         <v>4.19229999999515</v>
       </c>
-      <c r="M7" s="3">
+      <c r="M7" s="2">
         <v>1.1100001138402101E-2</v>
       </c>
-      <c r="N7" s="3">
+      <c r="N7" s="2">
         <v>0.79821101397326999</v>
       </c>
     </row>
     <row r="8" spans="1:15">
-      <c r="A8" s="4">
+      <c r="A8" s="3">
         <v>120</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="4">
         <v>11.9842500000959</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="4">
         <v>3.0250000854721199E-2</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="4">
         <v>0.32778476981187599</v>
       </c>
-      <c r="K8" s="4">
+      <c r="K8" s="3">
         <v>6000</v>
       </c>
-      <c r="L8" s="5">
+      <c r="L8" s="4">
         <v>5.1544500014279002</v>
       </c>
-      <c r="M8" s="5">
+      <c r="M8" s="4">
         <v>1.37000002723652E-2</v>
       </c>
-      <c r="N8" s="5">
+      <c r="N8" s="4">
         <v>0.57105539295076702</v>
       </c>
     </row>
     <row r="9" spans="1:15">
-      <c r="A9" s="2">
+      <c r="A9" s="1">
         <v>140</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="2">
         <v>15.3880999991088</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="2">
         <v>3.66000000212807E-2</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="2">
         <v>0.32716487407422801</v>
       </c>
-      <c r="K9" s="2">
+      <c r="K9" s="1">
         <v>7000</v>
       </c>
-      <c r="L9" s="3">
+      <c r="L9" s="2">
         <v>6.8236500000057196</v>
       </c>
-      <c r="M9" s="3">
+      <c r="M9" s="2">
         <v>1.1900000390596599E-2</v>
       </c>
-      <c r="N9" s="3">
+      <c r="N9" s="2">
         <v>0.52839189187523505</v>
       </c>
     </row>
     <row r="10" spans="1:15">
-      <c r="A10" s="4">
+      <c r="A10" s="3">
         <v>160</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="4">
         <v>17.8955499996664</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="4">
         <v>4.0250000602100003E-2</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="4">
         <v>0.26511055390927202</v>
       </c>
-      <c r="K10" s="4">
+      <c r="K10" s="3">
         <v>8000</v>
       </c>
-      <c r="L10" s="5">
+      <c r="L10" s="4">
         <v>7.3581000001286103</v>
       </c>
-      <c r="M10" s="5">
+      <c r="M10" s="4">
         <v>1.22499999997671E-2</v>
       </c>
-      <c r="N10" s="5">
+      <c r="N10" s="4">
         <v>0.49234639194933599</v>
       </c>
     </row>
     <row r="11" spans="1:15">
-      <c r="A11" s="2">
+      <c r="A11" s="1">
         <v>180</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="2">
         <v>20.198250000248599</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="2">
         <v>4.7549999871989698E-2</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="2">
         <v>0.27558426464982799</v>
       </c>
-      <c r="K11" s="2">
+      <c r="K11" s="1">
         <v>9000</v>
       </c>
-      <c r="L11" s="3">
+      <c r="L11" s="2">
         <v>8.6345500004244897</v>
       </c>
-      <c r="M11" s="3">
+      <c r="M11" s="2">
         <v>1.2299999652896E-2</v>
       </c>
-      <c r="N11" s="3">
+      <c r="N11" s="2">
         <v>0.27560970533096801</v>
       </c>
     </row>
     <row r="12" spans="1:15">
-      <c r="A12" s="4">
+      <c r="A12" s="3">
         <v>200</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B12" s="4">
         <v>22.433399999863401</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="4">
         <v>5.1450000173644997E-2</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="4">
         <v>0.242788361712546</v>
       </c>
-      <c r="K12" s="4">
+      <c r="K12" s="3">
         <v>10000</v>
       </c>
-      <c r="L12" s="5">
+      <c r="L12" s="4">
         <v>8.4979999999632092</v>
       </c>
-      <c r="M12" s="5">
+      <c r="M12" s="4">
         <v>1.1849999282276201E-2</v>
       </c>
-      <c r="N12" s="5">
+      <c r="N12" s="4">
         <v>0.32604193095828699</v>
       </c>
     </row>
     <row r="13" spans="1:15">
-      <c r="A13" s="2">
+      <c r="A13" s="1">
         <v>220</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="2">
         <v>24.728100000502302</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="2">
         <v>6.9700000312877805E-2</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="2">
         <v>0.21061251679191401</v>
       </c>
-      <c r="K13" s="2">
+      <c r="K13" s="1">
         <v>11000</v>
       </c>
-      <c r="L13" s="3">
+      <c r="L13" s="2">
         <v>13.2241999998223</v>
       </c>
-      <c r="M13" s="3">
+      <c r="M13" s="2">
         <v>1.21499998203944E-2</v>
       </c>
-      <c r="N13" s="3">
+      <c r="N13" s="2">
         <v>0.356123509923436</v>
       </c>
     </row>
     <row r="14" spans="1:15">
-      <c r="A14" s="4">
+      <c r="A14" s="3">
         <v>240</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B14" s="4">
         <v>27.092950000369399</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="4">
         <v>6.7200000194134094E-2</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="4">
         <v>0.220020296238047</v>
       </c>
-      <c r="K14" s="4">
+      <c r="K14" s="3">
         <v>12000</v>
       </c>
-      <c r="L14" s="5">
+      <c r="L14" s="4">
         <v>13.923500000382701</v>
       </c>
-      <c r="M14" s="5">
+      <c r="M14" s="4">
         <v>1.28499991842545E-2</v>
       </c>
-      <c r="N14" s="5">
+      <c r="N14" s="4">
         <v>0.30642212704315402</v>
       </c>
     </row>
     <row r="15" spans="1:15">
-      <c r="A15" s="2">
+      <c r="A15" s="1">
         <v>260</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="2">
         <v>29.540449998894399</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="2">
         <v>6.7150000249966896E-2</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15" s="2">
         <v>0.18618092081998699</v>
       </c>
-      <c r="K15" s="2">
+      <c r="K15" s="1">
         <v>13000</v>
       </c>
-      <c r="L15" s="3">
+      <c r="L15" s="2">
         <v>14.472050000331301</v>
       </c>
-      <c r="M15" s="3">
+      <c r="M15" s="2">
         <v>3.7899999879300497E-2</v>
       </c>
-      <c r="N15" s="3">
+      <c r="N15" s="2">
         <v>0.294454861039955</v>
       </c>
     </row>
     <row r="16" spans="1:15">
-      <c r="A16" s="4">
+      <c r="A16" s="3">
         <v>280</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B16" s="4">
         <v>31.572000000451201</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C16" s="4">
         <v>7.5950001482851803E-2</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16" s="4">
         <v>0.22340743237880101</v>
       </c>
-      <c r="K16" s="4">
+      <c r="K16" s="3">
         <v>14000</v>
       </c>
-      <c r="L16" s="5">
+      <c r="L16" s="4">
         <v>15.0382999997236</v>
       </c>
-      <c r="M16" s="5">
+      <c r="M16" s="4">
         <v>1.30499998340383E-2</v>
       </c>
-      <c r="N16" s="5">
+      <c r="N16" s="4">
         <v>0.240640107340265</v>
       </c>
     </row>
     <row r="17" spans="1:14">
-      <c r="A17" s="2">
+      <c r="A17" s="1">
         <v>300</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B17" s="2">
         <v>33.876850002561604</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17" s="2">
         <v>8.4549999446608098E-2</v>
       </c>
-      <c r="D17" s="3">
+      <c r="D17" s="2">
         <v>0.169973108295216</v>
       </c>
-      <c r="K17" s="2">
+      <c r="K17" s="1">
         <v>15000</v>
       </c>
-      <c r="L17" s="3">
+      <c r="L17" s="2">
         <v>16.133100000588399</v>
       </c>
-      <c r="M17" s="3">
+      <c r="M17" s="2">
         <v>1.3050000125076599E-2</v>
       </c>
-      <c r="N17" s="3">
+      <c r="N17" s="2">
         <v>0.23263963712485899</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix misslabeling of algos
</commit_message>
<xml_diff>
--- a/Wartości.xlsx
+++ b/Wartości.xlsx
@@ -414,11 +414,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="124929920"/>
-        <c:axId val="124940672"/>
+        <c:axId val="89868160"/>
+        <c:axId val="89878912"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="124929920"/>
+        <c:axId val="89868160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -443,14 +443,14 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="124940672"/>
+        <c:crossAx val="89878912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="124940672"/>
+        <c:axId val="89878912"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -481,7 +481,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="124929920"/>
+        <c:crossAx val="89868160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -494,7 +494,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -666,11 +666,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="124957056"/>
-        <c:axId val="124958976"/>
+        <c:axId val="89895296"/>
+        <c:axId val="89897216"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="124957056"/>
+        <c:axId val="89895296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -699,14 +699,14 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="124958976"/>
+        <c:crossAx val="89897216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="124958976"/>
+        <c:axId val="89897216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -737,7 +737,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="124957056"/>
+        <c:crossAx val="89895296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -750,7 +750,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1039,11 +1039,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="124423168"/>
-        <c:axId val="124425344"/>
+        <c:axId val="89558016"/>
+        <c:axId val="89568384"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="124423168"/>
+        <c:axId val="89558016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1073,14 +1073,14 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="124425344"/>
+        <c:crossAx val="89568384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="124425344"/>
+        <c:axId val="89568384"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1107,7 +1107,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="124423168"/>
+        <c:crossAx val="89558016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1120,7 +1120,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1279,11 +1279,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="124449536"/>
-        <c:axId val="124451456"/>
+        <c:axId val="90641536"/>
+        <c:axId val="90643456"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="124449536"/>
+        <c:axId val="90641536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1308,14 +1308,14 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="124451456"/>
+        <c:crossAx val="90643456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="124451456"/>
+        <c:axId val="90643456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1341,7 +1341,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="124449536"/>
+        <c:crossAx val="90641536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1354,7 +1354,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1772,8 +1772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O38" sqref="O38"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="D59" sqref="D59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>